<commit_message>
clean and sort out translators (sbml part done)
</commit_message>
<xml_diff>
--- a/examples/interaction_lists/Tcell_N3_PTEN2_interactions.xlsx
+++ b/examples/interaction_lists/Tcell_N3_PTEN2_interactions.xlsx
@@ -716,7 +716,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>FOS_DD</t>
+          <t>JUN</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -762,7 +762,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>JUN</t>
+          <t>FOS_DD</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -854,7 +854,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>NFKAPPAB</t>
+          <t>FOXP3</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -992,7 +992,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>AP1</t>
+          <t>NFKAPPAB</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -1038,7 +1038,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>FOXP3</t>
+          <t>AP1</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -1498,7 +1498,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>NFKAPPAB</t>
+          <t>NFAT</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -1544,7 +1544,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>NFAT</t>
+          <t>NFKAPPAB</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -1774,7 +1774,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>CD25</t>
+          <t>CD132</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -1820,7 +1820,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>CD132</t>
+          <t>CD25</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
@@ -1912,7 +1912,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>IL2R</t>
+          <t>IL2_EX</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
@@ -1958,7 +1958,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>IL2_EX</t>
+          <t>IL2R</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -2878,7 +2878,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>IL2R</t>
+          <t>CD28</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
@@ -2924,7 +2924,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>CD28</t>
+          <t>PI3K</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
@@ -3016,7 +3016,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>TCR</t>
+          <t>IL2R</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
@@ -3062,7 +3062,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>PI3K</t>
+          <t>TCR</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
@@ -3246,7 +3246,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>MTORC2</t>
+          <t>TCR</t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
@@ -3292,7 +3292,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>TCR</t>
+          <t>MTORC2</t>
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
@@ -3384,7 +3384,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>PTEN</t>
+          <t>FOXP3</t>
         </is>
       </c>
       <c r="B63" t="inlineStr"/>
@@ -3430,7 +3430,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>FOXP3</t>
+          <t>PTEN</t>
         </is>
       </c>
       <c r="B64" t="inlineStr"/>
@@ -3568,7 +3568,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>IL2R</t>
+          <t>CD28</t>
         </is>
       </c>
       <c r="B67" t="inlineStr"/>
@@ -3614,7 +3614,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>CD28</t>
+          <t>RAS</t>
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
@@ -3660,7 +3660,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>RAS</t>
+          <t>IL2_EX</t>
         </is>
       </c>
       <c r="B69" t="inlineStr"/>
@@ -3706,7 +3706,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>IL2_EX</t>
+          <t>IL2R</t>
         </is>
       </c>
       <c r="B70" t="inlineStr"/>

</xml_diff>

<commit_message>
clean and sort out translators (sbml-qual part done)
</commit_message>
<xml_diff>
--- a/examples/interaction_lists/Tcell_N3_PTEN2_interactions.xlsx
+++ b/examples/interaction_lists/Tcell_N3_PTEN2_interactions.xlsx
@@ -578,7 +578,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PDK1</t>
+          <t>MTORC2</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -624,7 +624,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MTORC2</t>
+          <t>PDK1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -854,7 +854,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>FOXP3</t>
+          <t>STAT5</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -900,7 +900,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>STAT5</t>
+          <t>NFAT</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -946,7 +946,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>NFAT</t>
+          <t>AP1</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -1038,7 +1038,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>AP1</t>
+          <t>FOXP3</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -1268,7 +1268,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>STAT5</t>
+          <t>MTOR_DD</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -1314,7 +1314,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>MTOR_DD</t>
+          <t>NFAT</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -1360,7 +1360,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>NFAT</t>
+          <t>SMAD3</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -1406,7 +1406,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>SMAD3</t>
+          <t>STAT5</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -1452,7 +1452,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>IL2</t>
+          <t>NFAT</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
@@ -1498,7 +1498,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>NFAT</t>
+          <t>NFKAPPAB</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -1544,7 +1544,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>NFKAPPAB</t>
+          <t>AP1</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -1590,7 +1590,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>AP1</t>
+          <t>IL2</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -1682,7 +1682,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>IL2</t>
+          <t>IL2_EX</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
@@ -1728,7 +1728,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>IL2_EX</t>
+          <t>IL2</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -1774,7 +1774,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>CD132</t>
+          <t>CD25</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -1820,7 +1820,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>CD25</t>
+          <t>CD122</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
@@ -1866,7 +1866,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>CD122</t>
+          <t>CD132</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
@@ -2878,7 +2878,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>CD28</t>
+          <t>TCR</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
@@ -2924,7 +2924,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>PI3K</t>
+          <t>CD28</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
@@ -2970,7 +2970,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>IL2_EX</t>
+          <t>PI3K</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
@@ -3016,7 +3016,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>IL2R</t>
+          <t>IL2_EX</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
@@ -3062,7 +3062,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>TCR</t>
+          <t>IL2R</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
@@ -3200,7 +3200,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>CD28</t>
+          <t>MTORC2</t>
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
@@ -3292,7 +3292,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>MTORC2</t>
+          <t>CD28</t>
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
@@ -3384,7 +3384,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>FOXP3</t>
+          <t>PTEN</t>
         </is>
       </c>
       <c r="B63" t="inlineStr"/>
@@ -3430,7 +3430,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>PTEN</t>
+          <t>FOXP3</t>
         </is>
       </c>
       <c r="B64" t="inlineStr"/>
@@ -3568,7 +3568,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>CD28</t>
+          <t>TCR</t>
         </is>
       </c>
       <c r="B67" t="inlineStr"/>
@@ -3614,7 +3614,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>RAS</t>
+          <t>CD28</t>
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
@@ -3660,7 +3660,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>IL2_EX</t>
+          <t>RAS</t>
         </is>
       </c>
       <c r="B69" t="inlineStr"/>
@@ -3706,7 +3706,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>IL2R</t>
+          <t>IL2_EX</t>
         </is>
       </c>
       <c r="B70" t="inlineStr"/>
@@ -3752,7 +3752,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>TCR</t>
+          <t>IL2R</t>
         </is>
       </c>
       <c r="B71" t="inlineStr"/>

</xml_diff>

<commit_message>
clean and sort out translators (sif part done)
</commit_message>
<xml_diff>
--- a/examples/interaction_lists/Tcell_N3_PTEN2_interactions.xlsx
+++ b/examples/interaction_lists/Tcell_N3_PTEN2_interactions.xlsx
@@ -900,7 +900,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>STAT5</t>
+          <t>FOXP3</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -992,7 +992,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>FOXP3</t>
+          <t>STAT5</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -1268,7 +1268,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>MTOR_DD</t>
+          <t>SMAD3</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -1314,7 +1314,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>NFAT</t>
+          <t>MTOR_DD</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -1360,7 +1360,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>SMAD3</t>
+          <t>NFAT</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -1544,7 +1544,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>IL2</t>
+          <t>NFKAPPAB</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -1590,7 +1590,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>NFKAPPAB</t>
+          <t>IL2</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -1774,7 +1774,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>CD25</t>
+          <t>CD122</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -1820,7 +1820,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>CD122</t>
+          <t>CD132</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
@@ -1866,7 +1866,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>CD132</t>
+          <t>CD25</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
@@ -1912,7 +1912,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>IL2_EX</t>
+          <t>IL2R</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
@@ -1958,7 +1958,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>IL2R</t>
+          <t>IL2_EX</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -2740,7 +2740,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>AKT</t>
+          <t>PKCTHETA</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
@@ -2786,7 +2786,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>PKCTHETA</t>
+          <t>AKT</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -2924,7 +2924,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>PI3K</t>
+          <t>TCR</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
@@ -2970,7 +2970,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>TCR</t>
+          <t>PI3K</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
@@ -3200,7 +3200,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>TCR</t>
+          <t>CD28</t>
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
@@ -3246,7 +3246,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>MTORC2</t>
+          <t>TCR</t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
@@ -3292,7 +3292,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>CD28</t>
+          <t>MTORC2</t>
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
@@ -3614,7 +3614,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>RAS</t>
+          <t>TCR</t>
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
@@ -3660,7 +3660,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>TCR</t>
+          <t>IL2_EX</t>
         </is>
       </c>
       <c r="B69" t="inlineStr"/>
@@ -3706,7 +3706,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>IL2_EX</t>
+          <t>IL2R</t>
         </is>
       </c>
       <c r="B70" t="inlineStr"/>
@@ -3752,7 +3752,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>IL2R</t>
+          <t>RAS</t>
         </is>
       </c>
       <c r="B71" t="inlineStr"/>

</xml_diff>